<commit_message>
Minor fixes to tables
</commit_message>
<xml_diff>
--- a/Figures and Tables/table1.xlsx
+++ b/Figures and Tables/table1.xlsx
@@ -25,10 +25,10 @@
     <t xml:space="preserve">Region</t>
   </si>
   <si>
-    <t xml:space="preserve">Difference in mortality rates (\%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">95 \% CI</t>
+    <t xml:space="preserve">Difference in mortality rates (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">95 % CI</t>
   </si>
   <si>
     <t xml:space="preserve">P Value</t>
@@ -233,12 +233,15 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.95"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>